<commit_message>
Change Type of hearing to Hearing type
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/data/non-strategic/ut-iac-judicial-review-daily-hearing-list/utIacJudicialReviewDailyHearingList.xlsx
+++ b/src/integrationTest/resources/data/non-strategic/ut-iac-judicial-review-daily-hearing-list/utIacJudicialReviewDailyHearingList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kian.kwa/IdeaProjects/pip-data-management/src/integrationTest/resources/data/non-strategic/ut-iac-judicial-review-daily-hearing-list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896DA4BF-D6EA-C140-8621-D0F1A1BAE184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2C3DF6-78EB-C04D-B4CC-26EA9474111F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51900" yWindow="1980" windowWidth="35140" windowHeight="26960" xr2:uid="{0C1F814A-B1E5-C24D-AA62-DAE35072E02F}"/>
   </bookViews>
@@ -71,9 +71,6 @@
     <t>representative</t>
   </si>
   <si>
-    <t>Type of hearing</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>11am</t>
+  </si>
+  <si>
+    <t>Hearing type</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,7 +485,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -500,10 +500,10 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -514,10 +514,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
       </c>
       <c r="D2">
         <v>1234</v>
@@ -526,7 +526,7 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -537,13 +537,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
       </c>
       <c r="D3">
         <v>1235</v>
@@ -552,7 +552,7 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Update test mock files
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/data/non-strategic/ut-iac-judicial-review-daily-hearing-list/utIacJudicialReviewDailyHearingList.xlsx
+++ b/src/integrationTest/resources/data/non-strategic/ut-iac-judicial-review-daily-hearing-list/utIacJudicialReviewDailyHearingList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kian.kwa/IdeaProjects/pip-data-management/src/integrationTest/resources/data/non-strategic/ut-iac-judicial-review-daily-hearing-list/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natasha.alker/Repos/pip/pip-data-management/src/integrationTest/resources/data/non-strategic/ut-iac-judicial-review-daily-hearing-list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2C3DF6-78EB-C04D-B4CC-26EA9474111F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAE91DB-C155-5A43-AA1B-2987734A7186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51900" yWindow="1980" windowWidth="35140" windowHeight="26960" xr2:uid="{0C1F814A-B1E5-C24D-AA62-DAE35072E02F}"/>
+    <workbookView xWindow="8160" yWindow="1280" windowWidth="35140" windowHeight="19520" xr2:uid="{0C1F814A-B1E5-C24D-AA62-DAE35072E02F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,24 +65,12 @@
     <t>Additional information</t>
   </si>
   <si>
-    <t>Applicant</t>
-  </si>
-  <si>
-    <t>representative</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
-    <t>Applicant A</t>
-  </si>
-  <si>
     <t>Rep A</t>
   </si>
   <si>
-    <t>Applicant B</t>
-  </si>
-  <si>
     <t>Rep B</t>
   </si>
   <si>
@@ -96,6 +84,18 @@
   </si>
   <si>
     <t>Hearing type</t>
+  </si>
+  <si>
+    <t>Case title</t>
+  </si>
+  <si>
+    <t>Representative</t>
+  </si>
+  <si>
+    <t>Case A</t>
+  </si>
+  <si>
+    <t>Case B</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,13 +485,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -500,10 +500,10 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -514,10 +514,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>1234</v>
@@ -526,7 +526,7 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -537,13 +537,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>1235</v>
@@ -552,7 +552,7 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Update common mock files for UT IAC JR regional lists
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/data/non-strategic/ut-iac-judicial-review-daily-hearing-list/utIacJudicialReviewDailyHearingList.xlsx
+++ b/src/integrationTest/resources/data/non-strategic/ut-iac-judicial-review-daily-hearing-list/utIacJudicialReviewDailyHearingList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kian.kwa/IdeaProjects/pip-data-management/src/integrationTest/resources/data/non-strategic/ut-iac-judicial-review-daily-hearing-list/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natasha.alker/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2C3DF6-78EB-C04D-B4CC-26EA9474111F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79584C7A-C89B-DD41-A3D6-6018A3DC58C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51900" yWindow="1980" windowWidth="35140" windowHeight="26960" xr2:uid="{0C1F814A-B1E5-C24D-AA62-DAE35072E02F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="19500" xr2:uid="{8B2F7226-3436-354A-9A19-EC024B5D6AA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,66 +36,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+  <si>
+    <t>Venue</t>
+  </si>
+  <si>
+    <t>Hearing time</t>
+  </si>
+  <si>
+    <t>Case reference number</t>
+  </si>
+  <si>
+    <t>Case title</t>
+  </si>
+  <si>
+    <t>Hearing type</t>
+  </si>
+  <si>
+    <t>Additional information</t>
+  </si>
+  <si>
+    <t>Venue A</t>
+  </si>
+  <si>
+    <t>Venue B</t>
+  </si>
+  <si>
+    <t>Venue C</t>
+  </si>
+  <si>
+    <t>Judge A</t>
+  </si>
+  <si>
+    <t>Judge B</t>
+  </si>
+  <si>
+    <t>Judge C</t>
+  </si>
+  <si>
+    <t>Case title A</t>
+  </si>
+  <si>
+    <t>Hearing type A</t>
+  </si>
+  <si>
+    <t>This is additional information</t>
+  </si>
+  <si>
+    <t>Case title B</t>
+  </si>
+  <si>
+    <t>Case title C</t>
+  </si>
+  <si>
+    <t>Hearing type B</t>
+  </si>
+  <si>
+    <t>Hearing type C</t>
+  </si>
   <si>
     <t>10:30am</t>
   </si>
   <si>
-    <t>Case reference number</t>
-  </si>
-  <si>
-    <t>Judge A</t>
-  </si>
-  <si>
-    <t>Judge B</t>
-  </si>
-  <si>
-    <t>This is a venue name</t>
-  </si>
-  <si>
-    <t>This is additional information</t>
-  </si>
-  <si>
-    <t>This is another additional information</t>
+    <t>11am</t>
+  </si>
+  <si>
+    <t>11:30am</t>
   </si>
   <si>
     <t>Judge(s)</t>
-  </si>
-  <si>
-    <t>Additional information</t>
-  </si>
-  <si>
-    <t>Applicant</t>
-  </si>
-  <si>
-    <t>representative</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Applicant A</t>
-  </si>
-  <si>
-    <t>Rep A</t>
-  </si>
-  <si>
-    <t>Applicant B</t>
-  </si>
-  <si>
-    <t>Rep B</t>
-  </si>
-  <si>
-    <t>Substantive</t>
-  </si>
-  <si>
-    <t>Hearing time</t>
-  </si>
-  <si>
-    <t>11am</t>
-  </si>
-  <si>
-    <t>Hearing type</t>
   </si>
 </sst>
 </file>
@@ -131,8 +140,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,99 +476,112 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B2781C7-F977-7445-AEF2-132F18114BDA}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B772A7FF-84F4-1943-87A8-12AED8F865C5}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.83203125" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" customWidth="1"/>
-    <col min="6" max="7" width="23.6640625" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="C2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
       </c>
       <c r="D2">
         <v>1234</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>4567</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>5678</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="F4" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G4" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3">
-        <v>1235</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>